<commit_message>
App is writing to xlsx but not to database and the values are missing
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,21 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>SKU</t>
   </si>
   <si>
     <t>Parent</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Closure</t>
   </si>
 </sst>
 </file>
@@ -386,30 +377,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:2">
       <c r="B2" t="b">
         <v>1</v>
       </c>

</xml_diff>